<commit_message>
Disable address search geocoder functionality in qgis2web.js and hide related UI elements in main.css; remove temporary Excel file.
</commit_message>
<xml_diff>
--- a/layers/ACVs_Municipality.xlsx
+++ b/layers/ACVs_Municipality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RyanDelacruz\Documents\Project_Tomas_New\layers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4D418F-6E78-4AB2-A947-249D470384A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EB2CCC-A2CA-4FF8-9128-01C62A77C977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3EFC6E2-DC33-4508-9255-B548EA67326B}"/>
   </bookViews>
@@ -548,9 +548,6 @@
     <t>BLS-CPR, SFA, WASAR</t>
   </si>
   <si>
-    <t>DELFIN ALBANO</t>
-  </si>
-  <si>
     <t>DELFIN ALBANO RESCUE TEAM 13 (DART 13)</t>
   </si>
   <si>
@@ -999,6 +996,9 @@
   </si>
   <si>
     <t>SAGUDAY</t>
+  </si>
+  <si>
+    <t>DELFIN ALBANO(MAGSAYSAY)</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD017176-BAAB-411A-B7A1-8016D8E56B53}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD69"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1504,7 +1504,7 @@
     <col min="3" max="9" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="54">
+    <row r="1" spans="1:9" ht="90">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2384,38 +2384,38 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18">
+    <row r="45" spans="1:9" ht="36">
       <c r="A45" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="H45" s="4">
         <v>18</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18">
       <c r="A46" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="47" spans="1:9" ht="18">
       <c r="A47" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2441,90 +2441,90 @@
     </row>
     <row r="48" spans="1:9" ht="18">
       <c r="A48" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="E48" s="4">
         <v>9184360268</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4">
         <v>87</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="18">
       <c r="A49" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="E49" s="4">
         <v>9772370357</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4">
         <v>14</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18">
       <c r="A50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="E50" s="4">
         <v>9065574826</v>
       </c>
       <c r="F50" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="H50" s="4">
         <v>52</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="18">
       <c r="A51" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="52" spans="1:9" ht="18">
       <c r="A52" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2550,11 +2550,11 @@
     </row>
     <row r="53" spans="1:9" ht="18">
       <c r="A53" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="54" spans="1:9" ht="18">
       <c r="A54" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2578,36 +2578,36 @@
     </row>
     <row r="55" spans="1:9" ht="18">
       <c r="A55" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="E55" s="4">
         <v>9359525634</v>
       </c>
       <c r="F55" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="H55" s="4">
         <v>24</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="18">
       <c r="A56" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="57" spans="1:9" ht="18">
       <c r="A57" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="58" spans="1:9" ht="18">
       <c r="A58" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2646,34 +2646,34 @@
     </row>
     <row r="59" spans="1:9" ht="18">
       <c r="A59" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="E59" s="12">
         <v>9392037768</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4">
         <v>15</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="18">
       <c r="A60" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="61" spans="1:9" ht="18">
       <c r="A61" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="62" spans="1:9" ht="18">
       <c r="A62" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2712,34 +2712,34 @@
     </row>
     <row r="63" spans="1:9" ht="18">
       <c r="A63" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="F63" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4">
         <v>5</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18">
       <c r="A64" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2752,34 +2752,34 @@
     </row>
     <row r="65" spans="1:9" ht="18">
       <c r="A65" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="F65" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4">
         <v>23</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="18">
       <c r="A66" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="67" spans="1:9" ht="18">
       <c r="A67" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="68" spans="1:9" ht="18">
       <c r="A68" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2818,20 +2818,20 @@
     </row>
     <row r="69" spans="1:9" ht="18">
       <c r="A69" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4">
@@ -2841,7 +2841,7 @@
     </row>
     <row r="70" spans="1:9" ht="18">
       <c r="A70" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="71" spans="1:9" ht="18">
       <c r="A71" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2867,22 +2867,22 @@
     </row>
     <row r="72" spans="1:9" ht="18">
       <c r="A72" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>253</v>
       </c>
       <c r="G72" s="4">
         <v>151.04</v>
@@ -2891,39 +2891,39 @@
         <v>54</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="18">
       <c r="A73" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="F73" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>260</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4">
         <v>34</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="18">
+      <c r="A74" s="14" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="36">
-      <c r="A74" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="75" spans="1:9" ht="18">
       <c r="A75" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2949,36 +2949,36 @@
     </row>
     <row r="76" spans="1:9" ht="18">
       <c r="A76" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="E76" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="G76" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="G76" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="H76" s="15">
         <v>34</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18">
       <c r="A77" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -2991,22 +2991,22 @@
     </row>
     <row r="78" spans="1:9" ht="18">
       <c r="A78" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="E78" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="F78" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>278</v>
       </c>
       <c r="G78" s="4">
         <v>148.45500000000001</v>
@@ -3015,18 +3015,18 @@
         <v>19</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18">
       <c r="A79" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="C79" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>282</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="80" spans="1:9" ht="18">
       <c r="A80" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -3050,22 +3050,22 @@
     </row>
     <row r="81" spans="1:9" ht="18">
       <c r="A81" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="C81" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="D81" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="E81" s="17">
         <v>9176589565</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G81" s="17">
         <v>151.85</v>
@@ -3074,27 +3074,27 @@
         <v>26</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18">
       <c r="A82" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="C82" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="D82" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="E82" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="E82" s="15" t="s">
+      <c r="F82" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="G82" s="17">
         <v>142.15</v>
@@ -3103,12 +3103,12 @@
         <v>19</v>
       </c>
       <c r="I82" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="18">
       <c r="A83" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="84" spans="1:9" ht="18">
       <c r="A84" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="85" spans="1:9" ht="18">
       <c r="A85" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -3147,7 +3147,7 @@
     </row>
     <row r="86" spans="1:9" ht="18">
       <c r="A86" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="87" spans="1:9" ht="18">
       <c r="A87" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -3173,22 +3173,22 @@
     </row>
     <row r="88" spans="1:9" ht="18">
       <c r="A88" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="E88" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="E88" s="20" t="s">
+      <c r="F88" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>306</v>
       </c>
       <c r="G88" s="4">
         <v>151.05000000000001</v>
@@ -3197,12 +3197,12 @@
         <v>10</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="18">
       <c r="A89" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="90" spans="1:9" ht="18">
       <c r="A90" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="91" spans="1:9" ht="18">
       <c r="A91" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="92" spans="1:9" ht="18">
       <c r="A92" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -3254,36 +3254,36 @@
     </row>
     <row r="93" spans="1:9" ht="18">
       <c r="A93" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B93" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="C93" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="D93" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="E93" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="E93" s="15" t="s">
+      <c r="F93" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="G93" s="15" t="s">
         <v>317</v>
-      </c>
-      <c r="G93" s="15" t="s">
-        <v>318</v>
       </c>
       <c r="H93" s="15">
         <v>52</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18">
       <c r="A94" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>

</xml_diff>

<commit_message>
Update ACVs_Municipality.xlsx with new data
</commit_message>
<xml_diff>
--- a/layers/ACVs_Municipality.xlsx
+++ b/layers/ACVs_Municipality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RyanDelacruz\Documents\Project_Tomas_New\layers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EB2CCC-A2CA-4FF8-9128-01C62A77C977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A9BF9-95FB-4705-B28E-664162642DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3EFC6E2-DC33-4508-9255-B548EA67326B}"/>
   </bookViews>
@@ -998,7 +998,7 @@
     <t>SAGUDAY</t>
   </si>
   <si>
-    <t>DELFIN ALBANO(MAGSAYSAY)</t>
+    <t>DELFIN ALBANO (MAGSAYSAY)</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1499,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="9" width="33.140625" customWidth="1"/>
   </cols>

</xml_diff>